<commit_message>
'#' will be ignored, and an empty message aborts the commit.
</commit_message>
<xml_diff>
--- a/每日支出详细.xlsx
+++ b/每日支出详细.xlsx
@@ -15,8 +15,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="F5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+万达广场，烤猪肉盖饭</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>日期</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -27,10 +63,6 @@
   </si>
   <si>
     <t>中饭</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>午饭</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -49,12 +81,27 @@
     <t>支出项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>晚饭</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚饭（干锅盔）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月总计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="179" formatCode="yyyy/m/d;@"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +133,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +159,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +224,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -176,22 +244,172 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -481,55 +699,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:Y38"/>
+  <dimension ref="B2:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
+    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
     <col min="4" max="6" width="9" style="1"/>
     <col min="7" max="7" width="12.25" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25">
+    <row r="2" spans="2:24">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-    </row>
-    <row r="3" spans="2:25">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+    </row>
+    <row r="3" spans="2:24">
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
       <c r="D3" s="2" t="s">
@@ -539,15 +758,17 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -563,19 +784,16 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-    </row>
-    <row r="4" spans="2:25">
-      <c r="B4" s="3">
-        <v>11.29</v>
+    </row>
+    <row r="4" spans="2:24">
+      <c r="B4" s="10">
+        <v>42703</v>
       </c>
       <c r="C4" s="3">
-        <f>SUM(D4:CO4)</f>
+        <f>SUM(D4:CN4)</f>
         <v>145</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3">
         <v>15</v>
       </c>
@@ -602,17 +820,25 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-    </row>
-    <row r="5" spans="2:25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+    </row>
+    <row r="5" spans="2:24">
+      <c r="B5" s="10">
+        <v>42704</v>
+      </c>
+      <c r="C5" s="3">
+        <f>SUM(D5:CN5)</f>
+        <v>35</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>32</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -628,17 +854,21 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-    </row>
-    <row r="6" spans="2:25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+    </row>
+    <row r="6" spans="2:24">
+      <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="12">
+        <f>SUM(C4:C5)</f>
+        <v>180</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -654,11 +884,15 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-    </row>
-    <row r="7" spans="2:25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+    </row>
+    <row r="7" spans="2:24">
+      <c r="B7" s="10">
+        <v>42705</v>
+      </c>
+      <c r="C7" s="3">
+        <f>SUM(D7:CN7)</f>
+        <v>0</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -680,11 +914,15 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-    </row>
-    <row r="8" spans="2:25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+    </row>
+    <row r="8" spans="2:24">
+      <c r="B8" s="10">
+        <v>42706</v>
+      </c>
+      <c r="C8" s="3">
+        <f>SUM(D8:CN8)</f>
+        <v>0</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -706,11 +944,15 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-    </row>
-    <row r="9" spans="2:25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+    </row>
+    <row r="9" spans="2:24">
+      <c r="B9" s="10">
+        <v>42707</v>
+      </c>
+      <c r="C9" s="3">
+        <f>SUM(D9:CN9)</f>
+        <v>0</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -732,11 +974,15 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-    </row>
-    <row r="10" spans="2:25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+    </row>
+    <row r="10" spans="2:24">
+      <c r="B10" s="10">
+        <v>42708</v>
+      </c>
+      <c r="C10" s="3">
+        <f>SUM(D10:CN10)</f>
+        <v>0</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -758,11 +1004,15 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-    </row>
-    <row r="11" spans="2:25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+    </row>
+    <row r="11" spans="2:24">
+      <c r="B11" s="10">
+        <v>42709</v>
+      </c>
+      <c r="C11" s="3">
+        <f>SUM(D11:CN11)</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -784,11 +1034,15 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-    </row>
-    <row r="12" spans="2:25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+    </row>
+    <row r="12" spans="2:24">
+      <c r="B12" s="10">
+        <v>42710</v>
+      </c>
+      <c r="C12" s="3">
+        <f>SUM(D12:CN12)</f>
+        <v>0</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -810,11 +1064,15 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-    </row>
-    <row r="13" spans="2:25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+    </row>
+    <row r="13" spans="2:24">
+      <c r="B13" s="10">
+        <v>42711</v>
+      </c>
+      <c r="C13" s="3">
+        <f>SUM(D13:CN13)</f>
+        <v>0</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -836,11 +1094,15 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-    </row>
-    <row r="14" spans="2:25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+    </row>
+    <row r="14" spans="2:24">
+      <c r="B14" s="10">
+        <v>42712</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(D14:CN14)</f>
+        <v>0</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -862,11 +1124,15 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-    </row>
-    <row r="15" spans="2:25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+    </row>
+    <row r="15" spans="2:24">
+      <c r="B15" s="10">
+        <v>42713</v>
+      </c>
+      <c r="C15" s="3">
+        <f>SUM(D15:CN15)</f>
+        <v>0</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -888,11 +1154,15 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-    </row>
-    <row r="16" spans="2:25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+    </row>
+    <row r="16" spans="2:24">
+      <c r="B16" s="10">
+        <v>42714</v>
+      </c>
+      <c r="C16" s="3">
+        <f>SUM(D16:CN16)</f>
+        <v>0</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -914,11 +1184,15 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-    </row>
-    <row r="17" spans="2:25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+    </row>
+    <row r="17" spans="2:24">
+      <c r="B17" s="10">
+        <v>42715</v>
+      </c>
+      <c r="C17" s="3">
+        <f>SUM(D17:CN17)</f>
+        <v>0</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -940,11 +1214,15 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-    </row>
-    <row r="18" spans="2:25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+    </row>
+    <row r="18" spans="2:24">
+      <c r="B18" s="10">
+        <v>42716</v>
+      </c>
+      <c r="C18" s="3">
+        <f>SUM(D18:CN18)</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -966,11 +1244,15 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-    </row>
-    <row r="19" spans="2:25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+    </row>
+    <row r="19" spans="2:24">
+      <c r="B19" s="10">
+        <v>42717</v>
+      </c>
+      <c r="C19" s="3">
+        <f>SUM(D19:CN19)</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -992,11 +1274,15 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-    </row>
-    <row r="20" spans="2:25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+    </row>
+    <row r="20" spans="2:24">
+      <c r="B20" s="10">
+        <v>42718</v>
+      </c>
+      <c r="C20" s="3">
+        <f>SUM(D20:CN20)</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1018,11 +1304,15 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-    </row>
-    <row r="21" spans="2:25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+    </row>
+    <row r="21" spans="2:24">
+      <c r="B21" s="10">
+        <v>42719</v>
+      </c>
+      <c r="C21" s="3">
+        <f>SUM(D21:CN21)</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1044,11 +1334,15 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-    </row>
-    <row r="22" spans="2:25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+    </row>
+    <row r="22" spans="2:24">
+      <c r="B22" s="10">
+        <v>42720</v>
+      </c>
+      <c r="C22" s="3">
+        <f>SUM(D22:CN22)</f>
+        <v>0</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1070,11 +1364,15 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-    </row>
-    <row r="23" spans="2:25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+    </row>
+    <row r="23" spans="2:24">
+      <c r="B23" s="10">
+        <v>42721</v>
+      </c>
+      <c r="C23" s="3">
+        <f>SUM(D23:CN23)</f>
+        <v>0</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1096,11 +1394,15 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-    </row>
-    <row r="24" spans="2:25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+    </row>
+    <row r="24" spans="2:24">
+      <c r="B24" s="10">
+        <v>42722</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(D24:CN24)</f>
+        <v>0</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1122,11 +1424,15 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-    </row>
-    <row r="25" spans="2:25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+    </row>
+    <row r="25" spans="2:24">
+      <c r="B25" s="10">
+        <v>42723</v>
+      </c>
+      <c r="C25" s="3">
+        <f>SUM(D25:CN25)</f>
+        <v>0</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1148,11 +1454,15 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-    </row>
-    <row r="26" spans="2:25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+    </row>
+    <row r="26" spans="2:24">
+      <c r="B26" s="10">
+        <v>42724</v>
+      </c>
+      <c r="C26" s="3">
+        <f>SUM(D26:CN26)</f>
+        <v>0</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1174,11 +1484,15 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-    </row>
-    <row r="27" spans="2:25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+    </row>
+    <row r="27" spans="2:24">
+      <c r="B27" s="10">
+        <v>42725</v>
+      </c>
+      <c r="C27" s="3">
+        <f>SUM(D27:CN27)</f>
+        <v>0</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1200,11 +1514,15 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-    </row>
-    <row r="28" spans="2:25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+    </row>
+    <row r="28" spans="2:24">
+      <c r="B28" s="10">
+        <v>42726</v>
+      </c>
+      <c r="C28" s="3">
+        <f>SUM(D28:CN28)</f>
+        <v>0</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1226,11 +1544,15 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-    </row>
-    <row r="29" spans="2:25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+    </row>
+    <row r="29" spans="2:24">
+      <c r="B29" s="10">
+        <v>42727</v>
+      </c>
+      <c r="C29" s="3">
+        <f>SUM(D29:CN29)</f>
+        <v>0</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1252,11 +1574,15 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-    </row>
-    <row r="30" spans="2:25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+    </row>
+    <row r="30" spans="2:24">
+      <c r="B30" s="10">
+        <v>42728</v>
+      </c>
+      <c r="C30" s="3">
+        <f>SUM(D30:CN30)</f>
+        <v>0</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1278,11 +1604,15 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-    </row>
-    <row r="31" spans="2:25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+    </row>
+    <row r="31" spans="2:24">
+      <c r="B31" s="10">
+        <v>42729</v>
+      </c>
+      <c r="C31" s="3">
+        <f>SUM(D31:CN31)</f>
+        <v>0</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1304,11 +1634,15 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-    </row>
-    <row r="32" spans="2:25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+    </row>
+    <row r="32" spans="2:24">
+      <c r="B32" s="10">
+        <v>42730</v>
+      </c>
+      <c r="C32" s="3">
+        <f>SUM(D32:CN32)</f>
+        <v>0</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1330,11 +1664,15 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-    </row>
-    <row r="33" spans="2:25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+    </row>
+    <row r="33" spans="2:24">
+      <c r="B33" s="10">
+        <v>42731</v>
+      </c>
+      <c r="C33" s="3">
+        <f>SUM(D33:CN33)</f>
+        <v>0</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1356,11 +1694,15 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-    </row>
-    <row r="34" spans="2:25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+    </row>
+    <row r="34" spans="2:24">
+      <c r="B34" s="10">
+        <v>42732</v>
+      </c>
+      <c r="C34" s="3">
+        <f>SUM(D34:CN34)</f>
+        <v>0</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1382,11 +1724,15 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-    </row>
-    <row r="35" spans="2:25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+    </row>
+    <row r="35" spans="2:24">
+      <c r="B35" s="10">
+        <v>42733</v>
+      </c>
+      <c r="C35" s="3">
+        <f>SUM(D35:CN35)</f>
+        <v>0</v>
+      </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1408,11 +1754,15 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-    </row>
-    <row r="36" spans="2:25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+    </row>
+    <row r="36" spans="2:24">
+      <c r="B36" s="10">
+        <v>42734</v>
+      </c>
+      <c r="C36" s="3">
+        <f>SUM(D36:CN36)</f>
+        <v>0</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1434,11 +1784,15 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-    </row>
-    <row r="37" spans="2:25">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+    </row>
+    <row r="37" spans="2:24">
+      <c r="B37" s="10">
+        <v>42735</v>
+      </c>
+      <c r="C37" s="3">
+        <f>SUM(D37:CN37)</f>
+        <v>0</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1460,17 +1814,21 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-    </row>
-    <row r="38" spans="2:25">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+    </row>
+    <row r="38" spans="2:24">
+      <c r="B38" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="12">
+        <f>SUM(C7:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -1486,17 +1844,82 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
+    </row>
+    <row r="39" spans="2:24">
+      <c r="B39" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C39" s="3">
+        <f>SUM(D39:CN39)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+    </row>
+    <row r="40" spans="2:24">
+      <c r="B40" s="10">
+        <v>42737</v>
+      </c>
+      <c r="C40" s="3">
+        <f>SUM(D40:CN40)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:Y2"/>
+    <mergeCell ref="D2:X2"/>
     <mergeCell ref="C2:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D4:I5 D7:I37 D39:I40">
+    <cfRule type="containsBlanks" dxfId="0" priority="4">
+      <formula>LEN(TRIM(D4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>